<commit_message>
second file commited msexecel.xlsx
</commit_message>
<xml_diff>
--- a/msexecel.xlsx
+++ b/msexecel.xlsx
@@ -16,6 +16,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>hth</t>
+  </si>
+  <si>
+    <t>ht</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +345,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D4:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>